<commit_message>
Updated intermediate-ish xlsx file with new params to reflect xlsm.
</commit_message>
<xml_diff>
--- a/Regression/Scenarios/EmbeddingPython/config.xlsx
+++ b/Regression/Scenarios/EmbeddingPython/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="270" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="270" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
   <si>
     <t>Campaign_Filename</t>
   </si>
@@ -97,6 +97,12 @@
     <t>Start_Time</t>
   </si>
   <si>
+    <t>Default_Geography_Initial_Node_Population</t>
+  </si>
+  <si>
+    <t>Default_Geography_Torus_Size</t>
+  </si>
+  <si>
     <t>Age_Initialization_Distribution_Type</t>
   </si>
   <si>
@@ -169,6 +175,9 @@
     <t>x_Other_Mortality</t>
   </si>
   <si>
+    <t>Minimum_Adult_Age_Years</t>
+  </si>
+  <si>
     <t>Job_Node_Groups</t>
   </si>
   <si>
@@ -347,6 +356,9 @@
   </si>
   <si>
     <t>Enable_Spatial_Output</t>
+  </si>
+  <si>
+    <t>Report_Event_Recorder</t>
   </si>
 </sst>
 </file>
@@ -358,31 +370,31 @@
   </numFmts>
   <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Courier 10 Pitch"/>
+      <family val="0"/>
       <charset val="1"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -428,8 +440,14 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -447,16 +465,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
+      <selection activeCell="A20" activeCellId="1" pane="topLeft" sqref="A19:B19 A20"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8509803921569"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.0588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.0561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -587,6 +606,22 @@
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -605,28 +640,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A15" activeCellId="0" pane="topLeft" sqref="A15"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
+      <selection activeCell="A19" activeCellId="0" pane="topLeft" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -634,7 +670,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -642,39 +678,39 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -682,7 +718,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -690,7 +726,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -698,7 +734,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -706,7 +742,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -714,7 +750,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -722,7 +758,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -730,7 +766,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>40</v>
@@ -738,15 +774,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -754,10 +790,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -779,34 +823,35 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A19:B19 A4"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -814,7 +859,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -839,17 +884,18 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="B5" activeCellId="1" pane="topLeft" sqref="A19:B19 B5"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>0.1</v>
@@ -857,7 +903,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -865,23 +911,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -889,7 +935,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3.5</v>
@@ -897,7 +943,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -905,7 +951,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -913,7 +959,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.25" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -921,7 +967,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -929,7 +975,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -937,7 +983,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -945,7 +991,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -953,7 +999,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -961,15 +1007,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -977,7 +1023,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -985,15 +1031,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1001,23 +1047,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -1025,7 +1071,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
@@ -1033,7 +1079,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.001</v>
@@ -1041,7 +1087,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>60</v>
@@ -1049,7 +1095,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -1057,7 +1103,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -1065,23 +1111,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.1</v>
@@ -1089,7 +1135,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>60</v>
@@ -1097,7 +1143,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -1122,17 +1168,18 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="A19:B19 A6"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>1</v>
@@ -1140,23 +1187,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -1164,7 +1211,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -1172,7 +1219,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -1180,7 +1227,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1188,7 +1235,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1196,7 +1243,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -1204,7 +1251,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>2</v>
@@ -1226,20 +1273,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="A5" activeCellId="1" pane="topLeft" sqref="A19:B19 A5"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>1</v>
@@ -1247,7 +1295,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1255,7 +1303,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1263,9 +1311,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Various fixes for issue 245.
</commit_message>
<xml_diff>
--- a/Regression/Scenarios/EmbeddingPython/config.xlsx
+++ b/Regression/Scenarios/EmbeddingPython/config.xlsx
@@ -136,7 +136,7 @@
     <t>Demographics_Filename</t>
   </si>
   <si>
-    <t>../00_Default/demographics.json</t>
+    <t>demographics.json</t>
   </si>
   <si>
     <t>Enable_Aging</t>
@@ -468,7 +468,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A20" activeCellId="1" pane="topLeft" sqref="A19:B19 A20"/>
+      <selection activeCell="A20" activeCellId="0" pane="topLeft" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -643,7 +643,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A19" activeCellId="0" pane="topLeft" sqref="A19:B19"/>
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -823,7 +823,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="1" pane="topLeft" sqref="A19:B19 A4"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -884,7 +884,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="1" pane="topLeft" sqref="A19:B19 B5"/>
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="A19:B19 A6"/>
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
-      <selection activeCell="A5" activeCellId="1" pane="topLeft" sqref="A19:B19 A5"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>